<commit_message>
Mon Jul 26 22:26:50 EDT 2021
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mengyang/Documents/github/phono_net/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A991A9DD-E6D2-E544-94B1-3EE55F68A5ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C774D80-6DC3-5F41-8EEC-ABE9305D15F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23720" yWindow="7680" windowWidth="27640" windowHeight="16940" xr2:uid="{D1AF7897-7F28-6B4E-AAB5-950D35A2BA07}"/>
+    <workbookView xWindow="23120" yWindow="8540" windowWidth="27640" windowHeight="16940" xr2:uid="{D1AF7897-7F28-6B4E-AAB5-950D35A2BA07}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>all</t>
   </si>
@@ -45,13 +45,19 @@
     <t>S</t>
   </si>
   <si>
-    <t>replace_pos_&lt;50%</t>
-  </si>
-  <si>
-    <t>replace_pos_&gt;=50%</t>
-  </si>
-  <si>
     <t>delete/insert</t>
+  </si>
+  <si>
+    <t>GC</t>
+  </si>
+  <si>
+    <t>Simple</t>
+  </si>
+  <si>
+    <t>pos&lt;50%</t>
+  </si>
+  <si>
+    <t>pos&gt;=50%</t>
   </si>
 </sst>
 </file>
@@ -403,19 +409,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A27372-C939-D540-AEC9-BD6CE206C000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="4" max="4" width="18.6640625" customWidth="1"/>
-    <col min="5" max="5" width="20.5" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -426,10 +431,10 @@
         <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -443,13 +448,13 @@
         <v>1590</v>
       </c>
       <c r="D2">
-        <v>144</v>
+        <v>3952</v>
       </c>
       <c r="E2">
-        <v>50</v>
+        <v>522</v>
       </c>
       <c r="F2">
-        <v>3952</v>
+        <v>485</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -463,13 +468,13 @@
         <v>0.39</v>
       </c>
       <c r="D3">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E3">
+        <v>0.48</v>
+      </c>
+      <c r="F3">
         <v>0.51</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -483,13 +488,13 @@
         <v>6.1</v>
       </c>
       <c r="D4">
-        <v>2.0299999999999998</v>
+        <v>13.23</v>
       </c>
       <c r="E4">
-        <v>2.34</v>
+        <v>5.57</v>
       </c>
       <c r="F4">
-        <v>13.23</v>
+        <v>6.67</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -500,13 +505,78 @@
         <v>79.08</v>
       </c>
       <c r="D5">
-        <v>4.18</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>3.23</v>
+        <v>8.9</v>
       </c>
       <c r="F5">
+        <v>36.159999999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>9075</v>
+      </c>
+      <c r="C8">
+        <v>7742</v>
+      </c>
+      <c r="D8">
+        <v>6248</v>
+      </c>
+      <c r="E8">
+        <v>7233</v>
+      </c>
+      <c r="F8">
+        <v>6729</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>0.31</v>
+      </c>
+      <c r="C9">
+        <v>0.39</v>
+      </c>
+      <c r="D9">
         <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0.53</v>
+      </c>
+      <c r="F9">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>6.05</v>
+      </c>
+      <c r="C10">
+        <v>5.28</v>
+      </c>
+      <c r="D10">
+        <v>13.22</v>
+      </c>
+      <c r="E10">
+        <v>5.0199999999999996</v>
+      </c>
+      <c r="F10">
+        <v>5.47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mon Jul 26 23:18:23 EDT 2021
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mengyang/Documents/github/phono_net/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C774D80-6DC3-5F41-8EEC-ABE9305D15F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7FF674E-14E9-5C41-A5CB-0F731E9B991E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23120" yWindow="8540" windowWidth="27640" windowHeight="16940" xr2:uid="{D1AF7897-7F28-6B4E-AAB5-950D35A2BA07}"/>
+    <workbookView xWindow="3420" yWindow="8620" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{D1AF7897-7F28-6B4E-AAB5-950D35A2BA07}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="correlation" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
   <si>
     <t>all</t>
   </si>
@@ -58,6 +59,9 @@
   </si>
   <si>
     <t>pos&gt;=50%</t>
+  </si>
+  <si>
+    <t>delete_insert</t>
   </si>
 </sst>
 </file>
@@ -411,7 +415,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A27372-C939-D540-AEC9-BD6CE206C000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
@@ -582,4 +586,83 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3F65138-7F7A-9D44-AA00-4D4BC7BA4C8C}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>0.59</v>
+      </c>
+      <c r="C3">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>0.94</v>
+      </c>
+      <c r="C4">
+        <v>0.92</v>
+      </c>
+      <c r="D4">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>0.78</v>
+      </c>
+      <c r="C5">
+        <v>0.74</v>
+      </c>
+      <c r="D5">
+        <v>0.52</v>
+      </c>
+      <c r="E5">
+        <v>0.52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Tue Jul 27 14:59:07 EDT 2021
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mengyang/Documents/github/phono_net/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7FF674E-14E9-5C41-A5CB-0F731E9B991E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CBB3E88-16FD-6042-920E-919A7EB66020}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="8620" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{D1AF7897-7F28-6B4E-AAB5-950D35A2BA07}"/>
+    <workbookView xWindow="23040" yWindow="7880" windowWidth="27640" windowHeight="16940" xr2:uid="{D1AF7897-7F28-6B4E-AAB5-950D35A2BA07}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="14">
   <si>
     <t>all</t>
   </si>
@@ -52,9 +52,6 @@
     <t>GC</t>
   </si>
   <si>
-    <t>Simple</t>
-  </si>
-  <si>
     <t>pos&lt;50%</t>
   </si>
   <si>
@@ -62,6 +59,15 @@
   </si>
   <si>
     <t>delete_insert</t>
+  </si>
+  <si>
+    <t>all degree &gt;= 5 (3406 words):</t>
+  </si>
+  <si>
+    <t>4184 words:</t>
+  </si>
+  <si>
+    <t>All</t>
   </si>
 </sst>
 </file>
@@ -415,8 +421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A27372-C939-D540-AEC9-BD6CE206C000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -435,10 +441,10 @@
         <v>6</v>
       </c>
       <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
         <v>9</v>
-      </c>
-      <c r="F1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -520,7 +526,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -590,76 +596,150 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3F65138-7F7A-9D44-AA00-4D4BC7BA4C8C}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>0.97</v>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>0.59</v>
-      </c>
-      <c r="C3">
-        <v>0.37</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4">
-        <v>0.94</v>
+        <v>0.59</v>
       </c>
       <c r="C4">
-        <v>0.92</v>
-      </c>
-      <c r="D4">
-        <v>0.51</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>0.94</v>
+      </c>
+      <c r="C5">
+        <v>0.92</v>
+      </c>
+      <c r="D5">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>0.78</v>
+      </c>
+      <c r="C6">
+        <v>0.74</v>
+      </c>
+      <c r="D6">
+        <v>0.52</v>
+      </c>
+      <c r="E6">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
         <v>10</v>
       </c>
-      <c r="B5">
-        <v>0.78</v>
-      </c>
-      <c r="C5">
-        <v>0.74</v>
-      </c>
-      <c r="D5">
-        <v>0.52</v>
-      </c>
-      <c r="E5">
-        <v>0.52</v>
+      <c r="E13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15">
+        <v>0.54</v>
+      </c>
+      <c r="C15">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16">
+        <v>0.92</v>
+      </c>
+      <c r="C16">
+        <v>0.9</v>
+      </c>
+      <c r="D16">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17">
+        <v>0.72</v>
+      </c>
+      <c r="C17">
+        <v>0.66</v>
+      </c>
+      <c r="D17">
+        <v>0.47</v>
+      </c>
+      <c r="E17">
+        <v>0.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>